<commit_message>
refactoring batch runner and excel helper
</commit_message>
<xml_diff>
--- a/wikilenium-core/src/test/resources/InvalidTestBatch.xlsx
+++ b/wikilenium-core/src/test/resources/InvalidTestBatch.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4DD356-B18D-4EEA-AF57-EC3593BD7063}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01857E77-B7F8-438F-B33E-CED0B348D752}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,10 +78,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -373,7 +372,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1"/>

</xml_diff>